<commit_message>
Excel datos en clase, timepo de CPU
</commit_message>
<xml_diff>
--- a/Datos clase.xlsx
+++ b/Datos clase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC22\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC22\Documents\Analisis-de-algoritmo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43CFBB74-B6A0-4A06-B99A-54DA273401F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8100362-6F45-4030-9BF2-30C9B9949AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6E92CBA-52B2-4DFF-91C0-B465F30782D8}"/>
   </bookViews>
@@ -131,6 +131,1028 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$E$4:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1258</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>852</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>987</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>777</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$K$4:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5320840</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>244560</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>213300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>233980</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>216480</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>201220</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>243780</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>216900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>258640</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>269140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACAC-4AE0-8238-6ADD7773ECB3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1258327023"/>
+        <c:axId val="1258327503"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1258327023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1258327503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1258327503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1258327023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37D789F6-97F2-114B-9CB0-B08274D12D11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -433,7 +1455,7 @@
   <dimension ref="D3:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,8 +1509,8 @@
         <v>5490100</v>
       </c>
       <c r="K4" s="1">
-        <f>AVERAGE(F4+G4+H4+I4+J4)</f>
-        <v>26604200</v>
+        <f>AVERAGE(F4:J4)</f>
+        <v>5320840</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
@@ -514,8 +1536,8 @@
         <v>183300</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" ref="K5:K13" si="0">AVERAGE(F5+G5+H5+I5+J5)</f>
-        <v>1222800</v>
+        <f t="shared" ref="K5:K13" si="0">AVERAGE(F5:J5)</f>
+        <v>244560</v>
       </c>
     </row>
     <row r="6" spans="4:11" x14ac:dyDescent="0.25">
@@ -542,7 +1564,7 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" si="0"/>
-        <v>1066500</v>
+        <v>213300</v>
       </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.25">
@@ -569,7 +1591,7 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>1169900</v>
+        <v>233980</v>
       </c>
     </row>
     <row r="8" spans="4:11" x14ac:dyDescent="0.25">
@@ -596,7 +1618,7 @@
       </c>
       <c r="K8" s="1">
         <f t="shared" si="0"/>
-        <v>1082400</v>
+        <v>216480</v>
       </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
@@ -623,7 +1645,7 @@
       </c>
       <c r="K9" s="1">
         <f t="shared" si="0"/>
-        <v>1006100</v>
+        <v>201220</v>
       </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
@@ -650,7 +1672,7 @@
       </c>
       <c r="K10" s="1">
         <f t="shared" si="0"/>
-        <v>1218900</v>
+        <v>243780</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.25">
@@ -677,7 +1699,7 @@
       </c>
       <c r="K11" s="1">
         <f t="shared" si="0"/>
-        <v>1084500</v>
+        <v>216900</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
@@ -704,7 +1726,7 @@
       </c>
       <c r="K12" s="1">
         <f t="shared" si="0"/>
-        <v>1293200</v>
+        <v>258640</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
@@ -731,7 +1753,7 @@
       </c>
       <c r="K13" s="1">
         <f t="shared" si="0"/>
-        <v>1345700</v>
+        <v>269140</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
@@ -762,5 +1784,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>